<commit_message>
Modification cardinalité Organization.name 553c730d16f17ca4dfa71516ef8d02ce83ccf078
</commit_message>
<xml_diff>
--- a/ig/280-281-correction-noms-orga/StructureDefinition-ror-organization.xlsx
+++ b/ig/280-281-correction-noms-orga/StructureDefinition-ror-organization.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-01-16T13:40:25+00:00</t>
+    <t>2024-02-14T09:13:51+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1767,7 +1767,7 @@
     <t>Organization.name</t>
   </si>
   <si>
-    <t>raisonSociale (EJ) ou denominationEG (EG) ou nomOI (OI)</t>
+    <t>raisonSociale (EJ) ou denominationEG (EG) ou nomOI (OI) - Remarque : Décalage provisoire de la cardinalité par rapport au modèle d'exposition (1..1)</t>
   </si>
   <si>
     <t>A name associated with the organization.</t>
@@ -18979,7 +18979,7 @@
       </c>
       <c r="E154" s="2"/>
       <c r="F154" t="s" s="2">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G154" t="s" s="2">
         <v>80</v>

</xml_diff>